<commit_message>
topic modeling on new data conducted
</commit_message>
<xml_diff>
--- a/Groups info.xlsx
+++ b/Groups info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Исследования и наука\Вузы привлечение абитуриентов\pyUNI_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F177A8A-ABFA-40F0-94E8-53EEFCF513EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B7F3F3-EA25-4555-8285-F27359B52804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
   <si>
     <t>University</t>
   </si>
@@ -36,27 +36,18 @@
     <t>НИУ ВШЭ</t>
   </si>
   <si>
-    <t>ГУАП</t>
-  </si>
-  <si>
     <t>ИТМО</t>
   </si>
   <si>
     <t>ЛЭТИ</t>
   </si>
   <si>
-    <t>СЗГМУ</t>
-  </si>
-  <si>
     <t>СПбГУТ</t>
   </si>
   <si>
     <t>СПбПУ</t>
   </si>
   <si>
-    <t>Мемы</t>
-  </si>
-  <si>
     <t>Основная</t>
   </si>
   <si>
@@ -64,9 +55,6 @@
   </si>
   <si>
     <t>Поступление</t>
-  </si>
-  <si>
-    <t>Профком</t>
   </si>
   <si>
     <t>File Number</t>
@@ -413,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -428,7 +416,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -442,10 +430,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -453,10 +441,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -464,10 +452,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -475,10 +463,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -489,7 +477,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -500,7 +488,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -508,10 +496,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -519,10 +507,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -541,10 +529,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -552,10 +540,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -563,10 +551,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -574,10 +562,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -585,10 +573,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -596,153 +584,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>